<commit_message>
Harmonized terminology, cleanup, minor bugs
- Revised terminology (use type -> function type, construction type -> structure type, expand -> increment, selection -> pool, etc.) in all files and codes to harmonize with manuscript
- Fixed pools that are already above the stop_count from erroneously summarizing as having 1 increment iteration
- Fixed boxplot colors for the histogram buildup graphic (figure 2)
- Cleaned up the directories from old files
</commit_message>
<xml_diff>
--- a/data_input_and_ml_processing/dims_structure.xlsx
+++ b/data_input_and_ml_processing/dims_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Dropbox\-the research\2020 10 IIASA\MI_project\buildings_db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Dropbox\-the research\2020 10 IIASA\MI_project\git\MaterialIntensityEstimator\data_input_and_ml_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD618AD-BC4A-4A08-8975-47206FCCEA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E405E-34FF-41CE-A60A-C2B75C434F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4212" windowWidth="22320" windowHeight="13176" xr2:uid="{5860A4FA-2A30-4856-957A-F941D70ED25A}"/>
+    <workbookView xWindow="19260" yWindow="5340" windowWidth="12495" windowHeight="12150" xr2:uid="{5860A4FA-2A30-4856-957A-F941D70ED25A}"/>
   </bookViews>
   <sheets>
     <sheet name="dims_structure" sheetId="1" r:id="rId1"/>
@@ -63,24 +63,9 @@
     <t>R5.2</t>
   </si>
   <si>
-    <t>Use_type</t>
-  </si>
-  <si>
-    <t>Construction_type_subtype</t>
-  </si>
-  <si>
-    <t>Energy_efficiency</t>
-  </si>
-  <si>
     <t>quantification_method</t>
   </si>
   <si>
-    <t>use_short</t>
-  </si>
-  <si>
-    <t>const_short</t>
-  </si>
-  <si>
     <t>R5_32</t>
   </si>
   <si>
@@ -367,6 +352,21 @@
   </si>
   <si>
     <t>R32RUS</t>
+  </si>
+  <si>
+    <t>function_type</t>
+  </si>
+  <si>
+    <t>structure_type_subtype</t>
+  </si>
+  <si>
+    <t>energy_efficiency</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>structure</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9722881C-C8E7-448A-ABFE-E3F6F7BF16D9}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -903,57 +903,57 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="60">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -999,31 +999,31 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="I4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" ref="J4:J35" si="2">RIGHT(C4,LEN(C4)-4)&amp;"_"&amp;RIGHT(B4,LEN(B4)-3)</f>
@@ -1033,28 +1033,28 @@
     </row>
     <row r="5" spans="1:14">
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="I5" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
@@ -1063,28 +1063,28 @@
     </row>
     <row r="6" spans="1:14">
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="I6" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
@@ -1093,25 +1093,25 @@
     </row>
     <row r="7" spans="1:14">
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -1120,22 +1120,22 @@
     </row>
     <row r="8" spans="1:14">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -1144,19 +1144,19 @@
     </row>
     <row r="9" spans="1:14">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -1165,16 +1165,16 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -1183,16 +1183,16 @@
     </row>
     <row r="11" spans="1:14">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
@@ -1201,16 +1201,16 @@
     </row>
     <row r="12" spans="1:14">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
@@ -1219,16 +1219,16 @@
     </row>
     <row r="13" spans="1:14">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
@@ -1237,16 +1237,16 @@
     </row>
     <row r="14" spans="1:14">
       <c r="B14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -1255,16 +1255,16 @@
     </row>
     <row r="15" spans="1:14">
       <c r="B15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -1273,16 +1273,16 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
@@ -1291,16 +1291,16 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -1309,13 +1309,13 @@
     </row>
     <row r="18" spans="2:10">
       <c r="B18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
@@ -1324,13 +1324,13 @@
     </row>
     <row r="19" spans="2:10">
       <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="2"/>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="20" spans="2:10">
       <c r="B20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="2"/>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="21" spans="2:10">
       <c r="B21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="2"/>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="23" spans="2:10">
       <c r="B23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="24" spans="2:10">
       <c r="B24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
@@ -1402,10 +1402,10 @@
     </row>
     <row r="25" spans="2:10">
       <c r="B25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
@@ -1414,10 +1414,10 @@
     </row>
     <row r="26" spans="2:10">
       <c r="B26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
@@ -1426,10 +1426,10 @@
     </row>
     <row r="27" spans="2:10">
       <c r="B27" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="2"/>
@@ -1438,10 +1438,10 @@
     </row>
     <row r="28" spans="2:10">
       <c r="B28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
@@ -1450,10 +1450,10 @@
     </row>
     <row r="29" spans="2:10">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="2"/>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="2"/>
@@ -1486,10 +1486,10 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="2"/>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="33" spans="2:10">
       <c r="B33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="2"/>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="34" spans="2:10">
       <c r="B34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="2"/>
@@ -1522,10 +1522,10 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="2"/>

</xml_diff>